<commit_message>
made more progress on project 2
</commit_message>
<xml_diff>
--- a/docs/ParseTable.xlsx
+++ b/docs/ParseTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="99" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t>Terminals</t>
   </si>
@@ -47,11 +47,26 @@
     <t>)</t>
   </si>
   <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
     <t>1. program</t>
   </si>
   <si>
     <r>
-      <t>program →</t>
+      <t xml:space="preserve">program →</t>
     </r>
     <r>
       <rPr>
@@ -62,7 +77,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>program id (</t>
+      <t xml:space="preserve">program id (</t>
     </r>
     <r>
       <rPr>
@@ -72,7 +87,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>identifier_list</t>
+      <t xml:space="preserve">identifier_list</t>
     </r>
     <r>
       <rPr>
@@ -83,7 +98,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>);</t>
+      <t xml:space="preserve">);</t>
     </r>
     <r>
       <rPr>
@@ -93,7 +108,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>program1</t>
+      <t xml:space="preserve">program1</t>
     </r>
   </si>
   <si>
@@ -104,7 +119,7 @@
   </si>
   <si>
     <r>
-      <t>program1 → subprogram_declarations compound_statement</t>
+      <t xml:space="preserve">program1 → subprogram_declarations compound_statement</t>
     </r>
     <r>
       <rPr>
@@ -115,12 +130,12 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>program1 → compound_statement</t>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">program1 → compound_statement</t>
     </r>
     <r>
       <rPr>
@@ -131,7 +146,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>.</t>
+      <t xml:space="preserve">.</t>
     </r>
   </si>
   <si>
@@ -139,7 +154,7 @@
   </si>
   <si>
     <r>
-      <t>program1_1 →  subprogram_declarations compound_statement</t>
+      <t xml:space="preserve">program1_1 →  subprogram_declarations compound_statement</t>
     </r>
     <r>
       <rPr>
@@ -150,12 +165,12 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>program1_1 → compound_statement</t>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">program1_1 → compound_statement</t>
     </r>
     <r>
       <rPr>
@@ -166,7 +181,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>.</t>
+      <t xml:space="preserve">.</t>
     </r>
   </si>
   <si>
@@ -174,7 +189,7 @@
   </si>
   <si>
     <r>
-      <t>identifier_list →</t>
+      <t xml:space="preserve">identifier_list →</t>
     </r>
     <r>
       <rPr>
@@ -185,7 +200,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>id </t>
+      <t xml:space="preserve">id</t>
     </r>
     <r>
       <rPr>
@@ -195,7 +210,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>identifier_list1</t>
+      <t xml:space="preserve">identifier_list1</t>
     </r>
   </si>
   <si>
@@ -203,7 +218,7 @@
   </si>
   <si>
     <r>
-      <t>identifier_list1 →</t>
+      <t xml:space="preserve">identifier_list1 →</t>
     </r>
     <r>
       <rPr>
@@ -214,7 +229,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>, id </t>
+      <t xml:space="preserve">, id</t>
     </r>
     <r>
       <rPr>
@@ -224,12 +239,12 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>identifier_list1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>identifier_list1 →</t>
+      <t xml:space="preserve">identifier_list1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">identifier_list1 →</t>
     </r>
     <r>
       <rPr>
@@ -240,7 +255,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>epsilon</t>
+      <t xml:space="preserve">epsilon</t>
     </r>
   </si>
   <si>
@@ -248,7 +263,7 @@
   </si>
   <si>
     <r>
-      <t>declarations →</t>
+      <t xml:space="preserve">declarations →</t>
     </r>
     <r>
       <rPr>
@@ -259,7 +274,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>var id :</t>
+      <t xml:space="preserve">var id :</t>
     </r>
     <r>
       <rPr>
@@ -268,7 +283,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>type</t>
+      <t xml:space="preserve">type</t>
     </r>
     <r>
       <rPr>
@@ -279,7 +294,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>;</t>
+      <t xml:space="preserve">;</t>
     </r>
     <r>
       <rPr>
@@ -289,7 +304,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>declarations1</t>
+      <t xml:space="preserve">declarations1</t>
     </r>
   </si>
   <si>
@@ -297,7 +312,7 @@
   </si>
   <si>
     <r>
-      <t>declarations1 →</t>
+      <t xml:space="preserve">declarations1 →</t>
     </r>
     <r>
       <rPr>
@@ -308,7 +323,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>var id :</t>
+      <t xml:space="preserve">var id :</t>
     </r>
     <r>
       <rPr>
@@ -317,7 +332,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>type</t>
+      <t xml:space="preserve">type</t>
     </r>
     <r>
       <rPr>
@@ -328,7 +343,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>;</t>
+      <t xml:space="preserve">;</t>
     </r>
     <r>
       <rPr>
@@ -338,12 +353,12 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>declarations1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>declarations1 →</t>
+      <t xml:space="preserve">declarations1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">declarations1 →</t>
     </r>
     <r>
       <rPr>
@@ -353,7 +368,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>epsilon</t>
+      <t xml:space="preserve">epsilon</t>
     </r>
   </si>
   <si>
@@ -373,7 +388,7 @@
   </si>
   <si>
     <r>
-      <t>subprogram_declarations1 → subprogram_declaration</t>
+      <t xml:space="preserve">subprogram_declarations1 → subprogram_declaration</t>
     </r>
     <r>
       <rPr>
@@ -384,7 +399,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>;</t>
+      <t xml:space="preserve">;</t>
     </r>
     <r>
       <rPr>
@@ -394,12 +409,12 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>subprogram_declarations1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>subprogram_declarations1 →</t>
+      <t xml:space="preserve">subprogram_declarations1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">subprogram_declarations1 →</t>
     </r>
     <r>
       <rPr>
@@ -409,7 +424,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>epsilon</t>
+      <t xml:space="preserve">epsilon</t>
     </r>
   </si>
   <si>
@@ -429,7 +444,7 @@
   </si>
   <si>
     <r>
-      <t>subprogram_declaration1 →</t>
+      <t xml:space="preserve">subprogram_declaration1 →</t>
     </r>
     <r>
       <rPr>
@@ -439,7 +454,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>compound_statement</t>
+      <t xml:space="preserve">compound_statement</t>
     </r>
   </si>
   <si>
@@ -456,7 +471,7 @@
   </si>
   <si>
     <r>
-      <t>subprogram_head →</t>
+      <t xml:space="preserve">subprogram_head →</t>
     </r>
     <r>
       <rPr>
@@ -467,7 +482,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>function id</t>
+      <t xml:space="preserve">function id </t>
     </r>
     <r>
       <rPr>
@@ -477,25 +492,282 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t>subprogram_head1</t>
+      <t xml:space="preserve">subprogram_head1</t>
     </r>
   </si>
   <si>
     <t>8.1 subprogram_head1</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">subprogram_head → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">function id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">subprogram_head1</t>
+    </r>
+  </si>
+  <si>
     <t>9. parameter_list</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">parameter_list → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> : type parameter_list1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">subprogram_head1 → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> parameter_list </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">standard_type </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">subprogram_head1 → : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">standard_type </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">;</t>
+    </r>
+  </si>
+  <si>
     <t>9.1 parameter_list1</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">parameter_list1 → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">epsilon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">parameter_list1 → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">; id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> type parameter_list1</t>
+    </r>
+  </si>
+  <si>
     <t>10. compound_statement</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">compound_statement →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">begin </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">compound_statement1</t>
+    </r>
+  </si>
+  <si>
     <t>10.1 compound_statement1</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">compound_statement1 → statement_list </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">end</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">compound_statement1 → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12"/>
+        <color rgb="FF00000A"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">end</t>
+    </r>
+  </si>
+  <si>
     <t>11. statement_list</t>
   </si>
   <si>
@@ -503,6 +775,139 @@
   </si>
   <si>
     <t>12. statement</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statement → </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">compound_statement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">statement → variable </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">assignop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> expression</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statement → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">expression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> statement statement1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Statement → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> expression </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> statement</t>
+    </r>
   </si>
   <si>
     <t>12.1 statement1</t>
@@ -554,7 +959,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -602,6 +1007,33 @@
       <sz val="11"/>
       <color rgb="FF00000A"/>
       <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val=""/>
       <family val="1"/>
       <charset val="1"/>
     </font>
@@ -669,7 +1101,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -708,6 +1140,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -789,8 +1233,8 @@
   </sheetPr>
   <dimension ref="A1:BC39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -802,9 +1246,14 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.7857142857143"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.1938775510204"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.8214285714286"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.3673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="42.0969387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.1275510204082"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="50.2959183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="44.8724489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,11 +1289,21 @@
       <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -889,10 +1348,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -950,17 +1409,17 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1015,15 +1474,15 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1078,14 +1537,14 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1139,7 +1598,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1147,11 +1606,11 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="8" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1202,11 +1661,11 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1263,17 +1722,17 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="9" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1328,7 +1787,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1387,7 +1846,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1446,12 +1905,12 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1507,15 +1966,15 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1570,12 +2029,12 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1631,17 +2090,17 @@
     </row>
     <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1696,15 +2155,15 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1759,12 +2218,12 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1820,11 +2279,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1877,19 +2338,25 @@
       <c r="BB18" s="5"/>
       <c r="BC18" s="5"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="J19" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -1938,7 +2405,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1947,9 +2414,13 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="I20" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
+      <c r="K20" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -1997,12 +2468,14 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -2054,23 +2527,33 @@
       <c r="BB21" s="5"/>
       <c r="BC21" s="5"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="L22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -2115,20 +2598,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
@@ -2174,7 +2653,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2233,20 +2712,28 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
+      <c r="L25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -2292,7 +2779,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2351,7 +2838,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2410,7 +2897,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2469,7 +2956,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2528,7 +3015,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2587,7 +3074,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2646,7 +3133,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2705,7 +3192,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2764,7 +3251,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2823,7 +3310,7 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2882,7 +3369,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2941,7 +3428,7 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -3000,7 +3487,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -3059,7 +3546,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>

</xml_diff>

<commit_message>
Finished Parse Table. Resolved Dangling Else ambiguity with parse table decision
</commit_message>
<xml_diff>
--- a/docs/ParseTable.xlsx
+++ b/docs/ParseTable.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="127">
   <si>
     <t>Terminals</t>
   </si>
@@ -62,53 +62,92 @@
     <t>end</t>
   </si>
   <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>assignop</t>
+  </si>
+  <si>
+    <t>multop</t>
+  </si>
+  <si>
+    <t>addop</t>
+  </si>
+  <si>
+    <t>relop</t>
+  </si>
+  <si>
+    <t>then</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>"+” (plus)</t>
+  </si>
+  <si>
+    <t>“-” (minus)</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
     <t>1. program</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">program →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">program id (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">identifier_list</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">);</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">program1</t>
+      <t>program →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>program id (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>identifier_list</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>program1</t>
     </r>
   </si>
   <si>
@@ -119,34 +158,34 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">program1 → subprogram_declarations compound_statement</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">program1 → compound_statement</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
+      <t>program1 → subprogram_declarations compound_statement</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>program1 → compound_statement</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
   <si>
@@ -154,34 +193,34 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">program1_1 →  subprogram_declarations compound_statement</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">program1_1 → compound_statement</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
+      <t>program1_1 →  subprogram_declarations compound_statement</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>program1_1 → compound_statement</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
   <si>
@@ -189,28 +228,28 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">identifier_list →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">identifier_list1</t>
+      <t>identifier_list →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>identifier_list1</t>
     </r>
   </si>
   <si>
@@ -218,44 +257,44 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">identifier_list1 →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">, id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">identifier_list1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">identifier_list1 →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">epsilon</t>
+      <t>identifier_list1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>, id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>identifier_list1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>identifier_list1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>epsilon</t>
     </r>
   </si>
   <si>
@@ -263,18 +302,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">declarations →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">var id :</t>
+      <t>declarations →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>var id :</t>
     </r>
     <r>
       <rPr>
@@ -283,28 +322,28 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">type</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">declarations1</t>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>declarations1</t>
     </r>
   </si>
   <si>
@@ -312,18 +351,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">declarations1 →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">var id :</t>
+      <t>declarations1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>var id :</t>
     </r>
     <r>
       <rPr>
@@ -332,33 +371,33 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">type</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">declarations1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">declarations1 →</t>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>declarations1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>declarations1 →</t>
     </r>
     <r>
       <rPr>
@@ -368,7 +407,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">epsilon</t>
+      <t>epsilon</t>
     </r>
   </si>
   <si>
@@ -388,33 +427,33 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">subprogram_declarations1 → subprogram_declaration</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">subprogram_declarations1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">subprogram_declarations1 →</t>
+      <t>subprogram_declarations1 → subprogram_declaration</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>subprogram_declarations1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>subprogram_declarations1 →</t>
     </r>
     <r>
       <rPr>
@@ -424,7 +463,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">epsilon</t>
+      <t>epsilon</t>
     </r>
   </si>
   <si>
@@ -444,7 +483,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">subprogram_declaration1 →</t>
+      <t>subprogram_declaration1 →</t>
     </r>
     <r>
       <rPr>
@@ -454,7 +493,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">compound_statement</t>
+      <t>compound_statement</t>
     </r>
   </si>
   <si>
@@ -471,97 +510,76 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">subprogram_head →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">function id </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">subprogram_head1</t>
+      <t>subprogram_head →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>function id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>subprogram_head1</t>
     </r>
   </si>
   <si>
     <t>8.1 subprogram_head1</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">subprogram_head → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">function id </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">subprogram_head1</t>
-    </r>
-  </si>
-  <si>
     <t>9. parameter_list</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">parameter_list → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> : type parameter_list1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">subprogram_head1 → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
+      <t>parameter_list →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: type parameter_list1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>subprogram_head1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(</t>
     </r>
     <r>
       <rPr>
@@ -570,17 +588,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> parameter_list </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
+      <t>parameter_list</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>):</t>
     </r>
     <r>
       <rPr>
@@ -589,93 +608,263 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
+      <t>standard_type</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>subprogram_head1 → :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>standard_type</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>9.1 parameter_list1</t>
+  </si>
+  <si>
+    <r>
+      <t>parameter_list1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">standard_type </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">subprogram_head1 → : </t>
-    </r>
-    <r>
-      <rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>parameter_list1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>; id:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>type parameter_list1</t>
+    </r>
+  </si>
+  <si>
+    <t>10. compound_statement</t>
+  </si>
+  <si>
+    <r>
+      <t>compound_statement →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>begin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>compound_statement1</t>
+    </r>
+  </si>
+  <si>
+    <t>10.1 compound_statement1</t>
+  </si>
+  <si>
+    <r>
+      <t>compound_statement1 → statement_list</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>end</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>compound_statement1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">standard_type </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">;</t>
-    </r>
-  </si>
-  <si>
-    <t>9.1 parameter_list1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">parameter_list1 → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>end</t>
+    </r>
+  </si>
+  <si>
+    <t>11. statement_list</t>
+  </si>
+  <si>
+    <t>11.1 statement_list1</t>
+  </si>
+  <si>
+    <t>12. statement</t>
+  </si>
+  <si>
+    <r>
+      <t>Statement →</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>compound_statement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>statement → variable</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>assignop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>expression</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Statement →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>if</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">epsilon</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">parameter_list1 → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">; id</t>
+      <t>expression</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>statement statement1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Statement →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>while</t>
     </r>
     <r>
       <rPr>
@@ -684,201 +873,437 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> type parameter_list1</t>
-    </r>
-  </si>
-  <si>
-    <t>10. compound_statement</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">compound_statement →</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">begin </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">compound_statement1</t>
-    </r>
-  </si>
-  <si>
-    <t>10.1 compound_statement1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">compound_statement1 → statement_list </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">end</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">compound_statement1 → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="12"/>
-        <color rgb="FF00000A"/>
-        <rFont val=""/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">end</t>
-    </r>
-  </si>
-  <si>
-    <t>11. statement_list</t>
-  </si>
-  <si>
-    <t>11.1 statement_list1</t>
-  </si>
-  <si>
-    <t>12. statement</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Statement → </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">compound_statement</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">statement → variable </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">assignop</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> expression</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Statement → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">if </t>
-    </r>
-    <r>
-      <rPr>
+      <t>expression</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>do</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>statement</t>
+    </r>
+  </si>
+  <si>
+    <t>12.1 statement1</t>
+  </si>
+  <si>
+    <r>
+      <t>statement1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">expression</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> statement statement1 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Statement → </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">while</t>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>statement1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>else</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>statement</t>
+    </r>
+  </si>
+  <si>
+    <t>13. variable</t>
+  </si>
+  <si>
+    <r>
+      <t>variable →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>variable1</t>
+    </r>
+  </si>
+  <si>
+    <t>13.1 variable1</t>
+  </si>
+  <si>
+    <r>
+      <t>variable1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>variable1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>expression</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>variable1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <t>14. expression_list</t>
+  </si>
+  <si>
+    <t>expression_list →expression expression_list1</t>
+  </si>
+  <si>
+    <t>14.1 expression_list1</t>
+  </si>
+  <si>
+    <r>
+      <t>expression_list1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>expression</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>expression_list1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <t>15. expression</t>
+  </si>
+  <si>
+    <t>expression → simple_expression expression1</t>
+  </si>
+  <si>
+    <t>15.1 expression1</t>
+  </si>
+  <si>
+    <r>
+      <t>expression1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>expression1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>relop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>simple_expression</t>
+    </r>
+  </si>
+  <si>
+    <t>16. simple_expression</t>
+  </si>
+  <si>
+    <t>simple_expression → term simple_expression1</t>
+  </si>
+  <si>
+    <t>simple_expression → sign term simple_expression1</t>
+  </si>
+  <si>
+    <t>16.1 simple_expression1</t>
+  </si>
+  <si>
+    <r>
+      <t>simple_expression1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>simple_expression1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>addop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>term simple_expression1</t>
+    </r>
+  </si>
+  <si>
+    <t>17. term</t>
+  </si>
+  <si>
+    <t>term → factor term1</t>
+  </si>
+  <si>
+    <t>17. term1</t>
+  </si>
+  <si>
+    <r>
+      <t>term1 → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>term1 →</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>multop </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>factor term1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>term1 → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>epsilon</t>
+    </r>
+  </si>
+  <si>
+    <t>18. factor</t>
+  </si>
+  <si>
+    <r>
+      <t>factor → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>factor1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>factor → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
     </r>
     <r>
       <rPr>
@@ -887,69 +1312,130 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> expression </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">do</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> statement</t>
-    </r>
-  </si>
-  <si>
-    <t>12.1 statement1</t>
-  </si>
-  <si>
-    <t>13. variable</t>
-  </si>
-  <si>
-    <t>13.1 variable1</t>
-  </si>
-  <si>
-    <t>14. expression_list</t>
-  </si>
-  <si>
-    <t>14.1 expression_list1</t>
-  </si>
-  <si>
-    <t>15. expression</t>
-  </si>
-  <si>
-    <t>15.1 expression1</t>
-  </si>
-  <si>
-    <t>16. simple_expression</t>
-  </si>
-  <si>
-    <t>16.1 simple_expression1</t>
-  </si>
-  <si>
-    <t>17. term</t>
-  </si>
-  <si>
-    <t>17. term1</t>
-  </si>
-  <si>
-    <t>18. factor</t>
+      <t> expression </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Factor → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>num</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Factor → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>factor</t>
+    </r>
   </si>
   <si>
     <t>18.1 factor1</t>
   </si>
   <si>
+    <t>factor1 → variable1</t>
+  </si>
+  <si>
+    <r>
+      <t>factor1 → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>expression_list</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> )</t>
+    </r>
+  </si>
+  <si>
     <t>19. sign</t>
+  </si>
+  <si>
+    <r>
+      <t>sign → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sign → </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>-</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -959,7 +1445,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1011,6 +1497,35 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF00000A"/>
+      <name val="Liberation Serif;Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00000A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF00000A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF00000A"/>
@@ -1023,22 +1538,8 @@
       <name val="Liberation Serif;Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
-      <name val=""/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1049,6 +1550,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1101,7 +1608,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1142,16 +1649,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1233,8 +1752,12 @@
   </sheetPr>
   <dimension ref="A1:BC39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="X18" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="bottomRight" activeCell="Y39" activeCellId="0" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1244,16 +1767,29 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.6632653061225"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="85.3316326530612"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="49.7857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.1938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="45.1326530612245"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.8469387755102"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="56.8214285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.3673469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.9132653061224"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="42.0969387755102"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="41.1275510204082"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="50.2959183673469"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="44.8724489795918"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.4897959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.1173469387755"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.2040816326531"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.6122448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="47.1020408163265"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="34.2704081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="30.0408163265306"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="29.6173469387755"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="50.6326530612245"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="45.1326530612245"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="46.6785714285714"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="47.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1304,24 +1840,50 @@
       <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
+      <c r="O2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
       <c r="AI2" s="4"/>
@@ -1348,10 +1910,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1409,17 +1971,17 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="7" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -1474,15 +2036,15 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="7" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1537,14 +2099,14 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="8" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1598,7 +2160,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1606,11 +2168,11 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="8" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="8" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1661,11 +2223,11 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1722,17 +2284,17 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="9" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -1787,7 +2349,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1846,7 +2408,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1905,12 +2467,12 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="8" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1966,15 +2528,15 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="8" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -2029,12 +2591,12 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="8" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -2090,17 +2652,17 @@
     </row>
     <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="8" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -2155,15 +2717,15 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="8" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -2218,12 +2780,12 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="9" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -2279,12 +2841,12 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="9" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -2340,22 +2902,22 @@
     </row>
     <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="9" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="10" t="s">
-        <v>56</v>
+      <c r="H19" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="J19" s="11" t="s">
-        <v>57</v>
+      <c r="J19" s="10" t="s">
+        <v>69</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -2405,7 +2967,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2414,12 +2976,12 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="12" t="s">
-        <v>59</v>
+      <c r="I20" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="9" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -2468,13 +3030,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="9" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -2529,30 +3091,30 @@
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>64</v>
+      <c r="E22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="N22" s="10" t="s">
-        <v>65</v>
+      <c r="L22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2598,7 +3160,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2653,7 +3215,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2712,16 +3274,16 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -2729,10 +3291,10 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -2779,7 +3341,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2790,11 +3352,17 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="K26" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
+      <c r="N26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O26" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
@@ -2838,13 +3406,15 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -2897,30 +3467,56 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="G28" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
+      <c r="K28" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
+      <c r="N28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="R28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="S28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="T28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="U28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="V28" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="W28" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
       <c r="Z28" s="5"/>
@@ -2956,15 +3552,19 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
+      <c r="H29" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
@@ -2980,10 +3580,18 @@
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
       <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
+      <c r="X29" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y29" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z29" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA29" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
@@ -3015,16 +3623,20 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="G30" s="9" t="s">
+        <v>97</v>
+      </c>
       <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -3074,15 +3686,19 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
+      <c r="F31" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+      <c r="H31" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
@@ -3098,10 +3714,18 @@
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
+      <c r="X31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z31" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA31" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
       <c r="AD31" s="5"/>
@@ -3133,30 +3757,48 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
+      <c r="I32" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
+      <c r="K32" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
+      <c r="N32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
+      <c r="Q32" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
+      <c r="U32" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="V32" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="W32" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
@@ -3192,15 +3834,19 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="F33" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
+      <c r="H33" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
@@ -3216,10 +3862,18 @@
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
+      <c r="X33" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y33" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z33" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA33" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
       <c r="AD33" s="5"/>
@@ -3251,30 +3905,50 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
+      <c r="G34" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
+      <c r="I34" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="K34" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
+      <c r="N34" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
+      <c r="Q34" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="R34" s="5"/>
       <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
-      <c r="V34" s="5"/>
-      <c r="W34" s="5"/>
+      <c r="T34" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="U34" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="V34" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="W34" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="X34" s="5"/>
       <c r="Y34" s="5"/>
       <c r="Z34" s="5"/>
@@ -3310,15 +3984,19 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="F35" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
+      <c r="H35" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -3336,8 +4014,12 @@
       <c r="W35" s="5"/>
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
-      <c r="Z35" s="5"/>
-      <c r="AA35" s="5"/>
+      <c r="Z35" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA35" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
       <c r="AD35" s="5"/>
@@ -3369,7 +4051,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3380,19 +4062,37 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
+      <c r="K36" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="L36" s="5"/>
       <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
+      <c r="N36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
+      <c r="Q36" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
-      <c r="U36" s="5"/>
-      <c r="V36" s="5"/>
-      <c r="W36" s="5"/>
+      <c r="S36" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="T36" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="V36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="W36" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="X36" s="5"/>
       <c r="Y36" s="5"/>
       <c r="Z36" s="5"/>
@@ -3428,15 +4128,19 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+      <c r="F37" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="H37" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -3454,8 +4158,12 @@
       <c r="W37" s="5"/>
       <c r="X37" s="5"/>
       <c r="Y37" s="5"/>
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="5"/>
+      <c r="Z37" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA37" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="AB37" s="5"/>
       <c r="AC37" s="5"/>
       <c r="AD37" s="5"/>
@@ -3487,30 +4195,56 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
+      <c r="G38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
+      <c r="K38" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
+      <c r="N38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="P38" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q38" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="W38" s="5"/>
+      <c r="S38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="T38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="U38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="V38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="W38" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="X38" s="5"/>
       <c r="Y38" s="5"/>
       <c r="Z38" s="5"/>
@@ -3546,7 +4280,7 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -3570,8 +4304,12 @@
       <c r="U39" s="5"/>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
-      <c r="X39" s="5"/>
-      <c r="Y39" s="5"/>
+      <c r="X39" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y39" s="9" t="s">
+        <v>126</v>
+      </c>
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>

</xml_diff>

<commit_message>
fixed submission attempt 1 errors
</commit_message>
<xml_diff>
--- a/docs/ParseTable.xlsx
+++ b/docs/ParseTable.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="99" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="93" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ParseTable" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">ParseTable!$A:$A,ParseTable!$2:$2</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
@@ -427,7 +430,7 @@
   </si>
   <si>
     <r>
-      <t>type → </t>
+      <t>type →</t>
     </r>
     <r>
       <rPr>
@@ -437,7 +440,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>[ num .. num ] of </t>
+      <t>[ num .. num ] of</t>
     </r>
     <r>
       <rPr>
@@ -454,7 +457,7 @@
   </si>
   <si>
     <r>
-      <t>standard_type → </t>
+      <t>standard_type →</t>
     </r>
     <r>
       <rPr>
@@ -469,7 +472,7 @@
   </si>
   <si>
     <r>
-      <t>standard_type –&gt; </t>
+      <t>standard_type –&gt;</t>
     </r>
     <r>
       <rPr>
@@ -672,7 +675,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t> → :</t>
+      <t>→ :</t>
     </r>
     <r>
       <rPr>
@@ -843,39 +846,42 @@
   </si>
   <si>
     <r>
-      <t>statement_list1 = </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
+      <t>statement_list1 =</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t>statement statement_list1</t>
     </r>
   </si>
   <si>
     <r>
-      <t>statement_list1 = </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF00000A"/>
-        <rFont val="Liberation Serif;Times New Roman"/>
-        <family val="1"/>
+      <t>statement_list1 =</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF00000A"/>
+        <rFont val="Liberation Serif;Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t>epsilon</t>
     </r>
@@ -1557,7 +1563,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1628,19 +1634,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00000A"/>
-      <name val="Liberation Serif;Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1848,16 +1841,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:AD39"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G16" activeCellId="0" sqref="G16:L24"/>
+      <selection pane="bottomRight" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3549,9 +3542,9 @@
       <c r="AD39" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions headings="true" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.681944444444444" right="0.477083333333333" top="0.809027777777778" bottom="0.789583333333333" header="0.542361111111111" footer="0.522916666666667"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="10" pageOrder="overThenDown" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>